<commit_message>
update the cycle model
</commit_message>
<xml_diff>
--- a/bia/equation/bia_data.xlsx
+++ b/bia/equation/bia_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shi_zhongming/Documents/GitHub/cea-plugin-bia/bia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shi_zhongming/Documents/GitHub/cea-plugin-bia/bia/equation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7F2473-70BD-DC48-9DE8-E1B179D426AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67420211-86A5-C949-BB82-51B5212C8549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="3160" windowWidth="27640" windowHeight="16940" xr2:uid="{CF3DEF0F-91FB-1846-99BB-4025335B9F21}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{CF3DEF0F-91FB-1846-99BB-4025335B9F21}"/>
   </bookViews>
   <sheets>
     <sheet name="crop" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
-  <si>
-    <t>crop_type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>description</t>
   </si>
@@ -37,9 +34,6 @@
     <t>Chinese red spinach or amaranth leaves are nutritionally similar to Swiss chard, spinach and beetroot leaves, and offer a rich source of carotenoids, vitamin C, minerals and trace elements. The leaves also contain the amino acids methionine and lysine making them a great companion for rice which is deficient in lysine. https://zenxin.com.sg/store/fresh-produce/vegetables-fresh-produce/organic-bayam-spinach-red-150g-thailand</t>
   </si>
   <si>
-    <t>BayamRed</t>
-  </si>
-  <si>
     <t>dli_l</t>
   </si>
   <si>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>dli_u</t>
+  </si>
+  <si>
+    <t>AmaranthRed</t>
+  </si>
+  <si>
+    <t>type_crop</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -488,75 +488,75 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="170">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>22</v>
@@ -571,7 +571,7 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I2">
         <v>35</v>
@@ -586,13 +586,13 @@
         <v>0.6</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N2">
         <v>12</v>
       </c>
-      <c r="O2" t="s">
-        <v>10</v>
+      <c r="O2">
+        <v>12</v>
       </c>
       <c r="P2">
         <v>3</v>
@@ -601,10 +601,10 @@
         <v>4.5</v>
       </c>
       <c r="R2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="S2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T2">
         <v>8</v>

</xml_diff>

<commit_message>
crop profile script finished before debug
</commit_message>
<xml_diff>
--- a/bia/equation/bia_data.xlsx
+++ b/bia/equation/bia_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shi_zhongming/Documents/GitHub/cea-plugin-bia/bia/equation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876FBCBC-DB32-1A43-83B8-989DE10000DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBBC287-B95A-F04C-8C3C-71CDB1E07766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{CF3DEF0F-91FB-1846-99BB-4025335B9F21}"/>
+    <workbookView xWindow="14200" yWindow="500" windowWidth="11700" windowHeight="16940" activeTab="2" xr2:uid="{CF3DEF0F-91FB-1846-99BB-4025335B9F21}"/>
   </bookViews>
   <sheets>
     <sheet name="crop" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
   <si>
     <t>description</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>soil_sgd_sqm</t>
+  </si>
+  <si>
+    <t>Lettuce</t>
+  </si>
+  <si>
+    <t>LettuceRomaine</t>
   </si>
 </sst>
 </file>
@@ -593,17 +599,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79F5D7C-03A3-E547-BB27-3867A23F521A}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="25" max="25" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -716,7 +722,7 @@
         <v>30</v>
       </c>
       <c r="L2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M2">
         <v>7</v>
@@ -733,8 +739,8 @@
       <c r="Q2">
         <v>12</v>
       </c>
-      <c r="R2">
-        <v>12</v>
+      <c r="R2" t="s">
+        <v>6</v>
       </c>
       <c r="S2">
         <v>3</v>
@@ -753,6 +759,148 @@
       </c>
       <c r="X2">
         <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="68">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
+      <c r="L3">
+        <v>13</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>0.5</v>
+      </c>
+      <c r="P3">
+        <v>0.7</v>
+      </c>
+      <c r="Q3">
+        <v>14.4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>326</v>
+      </c>
+      <c r="V3">
+        <v>278</v>
+      </c>
+      <c r="W3">
+        <v>240</v>
+      </c>
+      <c r="X3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="68">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>45</v>
+      </c>
+      <c r="L4">
+        <v>13</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>0.7</v>
+      </c>
+      <c r="Q4">
+        <v>14.4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>4</v>
+      </c>
+      <c r="U4">
+        <v>241</v>
+      </c>
+      <c r="V4">
+        <v>343</v>
+      </c>
+      <c r="W4">
+        <v>413</v>
+      </c>
+      <c r="X4">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -763,12 +911,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C28D85-B064-F646-954A-277E8D659D34}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="5" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -840,6 +991,64 @@
         <v>0</v>
       </c>
       <c r="I2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>84.6</v>
+      </c>
+      <c r="F3">
+        <v>42.5</v>
+      </c>
+      <c r="G3">
+        <v>1.24</v>
+      </c>
+      <c r="H3">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I3">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>12.8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>84.6</v>
+      </c>
+      <c r="F4">
+        <v>42.5</v>
+      </c>
+      <c r="G4">
+        <v>1.24</v>
+      </c>
+      <c r="H4">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I4">
         <v>0.43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
four types of vegetables have been added, now testing
</commit_message>
<xml_diff>
--- a/bia/equation/bia_data.xlsx
+++ b/bia/equation/bia_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shi_zhongming/Documents/GitHub/cea-plugin-bia/bia/equation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBBC287-B95A-F04C-8C3C-71CDB1E07766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992850A8-CC81-FA4E-AEC5-E63F8040B8D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14200" yWindow="500" windowWidth="11700" windowHeight="16940" activeTab="2" xr2:uid="{CF3DEF0F-91FB-1846-99BB-4025335B9F21}"/>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{CF3DEF0F-91FB-1846-99BB-4025335B9F21}"/>
   </bookViews>
   <sheets>
     <sheet name="crop" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
   <si>
     <t>description</t>
   </si>
@@ -65,18 +65,6 @@
     <t>temp_opt_gro_l_c</t>
   </si>
   <si>
-    <t>temp_por_l_c</t>
-  </si>
-  <si>
-    <t>temp_por_u_c</t>
-  </si>
-  <si>
-    <t>cycl_l_day</t>
-  </si>
-  <si>
-    <t>cycl_u_day</t>
-  </si>
-  <si>
     <t>humd_l</t>
   </si>
   <si>
@@ -222,6 +210,27 @@
   </si>
   <si>
     <t>LettuceRomaine</t>
+  </si>
+  <si>
+    <t>BitterGourd</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>CaiXinHongKong</t>
+  </si>
+  <si>
+    <t>non_experiment_data_using_okra_as_a_replacement</t>
+  </si>
+  <si>
+    <t>unkown</t>
+  </si>
+  <si>
+    <t>MustardGreen</t>
+  </si>
+  <si>
+    <t>FlatMustardGreen</t>
   </si>
 </sst>
 </file>
@@ -599,10 +608,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79F5D7C-03A3-E547-BB27-3867A23F521A}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -610,10 +622,10 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -621,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
@@ -635,59 +647,47 @@
       <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="170">
+    </row>
+    <row r="2" spans="1:21" ht="170">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>22</v>
@@ -709,64 +709,52 @@
       <c r="G2">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
+      <c r="H2">
+        <v>12</v>
       </c>
       <c r="I2">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="K2">
-        <v>30</v>
-      </c>
-      <c r="L2">
+        <v>0.6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2">
         <v>12</v>
       </c>
-      <c r="M2">
-        <v>7</v>
-      </c>
-      <c r="N2">
-        <v>7</v>
+      <c r="N2" t="s">
+        <v>6</v>
       </c>
       <c r="O2">
-        <v>0.6</v>
-      </c>
-      <c r="P2" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>4.5</v>
       </c>
       <c r="Q2">
-        <v>12</v>
-      </c>
-      <c r="R2" t="s">
-        <v>6</v>
+        <v>265</v>
+      </c>
+      <c r="R2">
+        <v>129</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>334</v>
       </c>
       <c r="T2">
-        <v>4.5</v>
-      </c>
-      <c r="U2">
-        <v>265</v>
-      </c>
-      <c r="V2">
-        <v>129</v>
-      </c>
-      <c r="W2">
-        <v>334</v>
-      </c>
-      <c r="X2">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="68">
+    <row r="3" spans="1:21" ht="68">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -780,64 +768,52 @@
       <c r="G3">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
+      <c r="H3">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="K3">
-        <v>45</v>
+        <v>0.5</v>
       </c>
       <c r="L3">
-        <v>13</v>
+        <v>0.7</v>
       </c>
       <c r="M3">
-        <v>7</v>
-      </c>
-      <c r="N3">
-        <v>7</v>
+        <v>14.4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
       </c>
       <c r="O3">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="P3">
-        <v>0.7</v>
+        <v>4</v>
       </c>
       <c r="Q3">
-        <v>14.4</v>
-      </c>
-      <c r="R3" t="s">
-        <v>6</v>
+        <v>326</v>
+      </c>
+      <c r="R3">
+        <v>278</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>240</v>
       </c>
       <c r="T3">
-        <v>4</v>
-      </c>
-      <c r="U3">
-        <v>326</v>
-      </c>
-      <c r="V3">
-        <v>278</v>
-      </c>
-      <c r="W3">
-        <v>240</v>
-      </c>
-      <c r="X3">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="68">
+    <row r="4" spans="1:21" ht="68">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -851,56 +827,342 @@
       <c r="G4">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
       </c>
       <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>0.5</v>
+      </c>
+      <c r="L4">
+        <v>0.7</v>
+      </c>
+      <c r="M4">
+        <v>14.4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>241</v>
+      </c>
+      <c r="R4">
+        <v>343</v>
+      </c>
+      <c r="S4">
+        <v>413</v>
+      </c>
+      <c r="T4">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="85">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>32</v>
+      </c>
+      <c r="H5">
         <v>30</v>
       </c>
-      <c r="K4">
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>0.8</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>6.48</v>
+      </c>
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <v>0.8</v>
+      </c>
+      <c r="P5">
+        <v>1.2</v>
+      </c>
+      <c r="Q5">
+        <v>1147</v>
+      </c>
+      <c r="R5">
+        <v>1032</v>
+      </c>
+      <c r="S5">
+        <v>1438</v>
+      </c>
+      <c r="T5">
+        <v>899</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="68">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>106</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0.65</v>
+      </c>
+      <c r="L6">
+        <v>0.9</v>
+      </c>
+      <c r="M6">
+        <v>10.8</v>
+      </c>
+      <c r="N6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>6</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6">
+        <v>2824</v>
+      </c>
+      <c r="R6">
+        <v>218</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="68">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
         <v>45</v>
       </c>
-      <c r="L4">
-        <v>13</v>
-      </c>
-      <c r="M4">
-        <v>7</v>
-      </c>
-      <c r="N4">
-        <v>7</v>
-      </c>
-      <c r="O4">
-        <v>0.5</v>
-      </c>
-      <c r="P4">
-        <v>0.7</v>
-      </c>
-      <c r="Q4">
-        <v>14.4</v>
-      </c>
-      <c r="R4" t="s">
-        <v>6</v>
-      </c>
-      <c r="S4">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0.8</v>
+      </c>
+      <c r="L7">
+        <v>0.9</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>1.5</v>
+      </c>
+      <c r="P7">
         <v>2</v>
       </c>
-      <c r="T4">
-        <v>4</v>
-      </c>
-      <c r="U4">
-        <v>241</v>
-      </c>
-      <c r="V4">
-        <v>343</v>
-      </c>
-      <c r="W4">
-        <v>413</v>
-      </c>
-      <c r="X4">
-        <v>330</v>
+      <c r="Q7">
+        <v>6408</v>
+      </c>
+      <c r="R7">
+        <v>6287</v>
+      </c>
+      <c r="S7">
+        <v>5095</v>
+      </c>
+      <c r="T7">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="68">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>10340</v>
+      </c>
+      <c r="R8">
+        <v>13306</v>
+      </c>
+      <c r="S8">
+        <v>17325</v>
+      </c>
+      <c r="T8">
+        <v>7705</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="68">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0.8</v>
+      </c>
+      <c r="L9">
+        <v>0.9</v>
+      </c>
+      <c r="M9">
+        <v>12</v>
+      </c>
+      <c r="N9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>3.5</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>4995</v>
+      </c>
+      <c r="R9">
+        <v>10080</v>
+      </c>
+      <c r="S9">
+        <v>10417</v>
+      </c>
+      <c r="T9">
+        <v>2926</v>
       </c>
     </row>
   </sheetData>
@@ -911,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C28D85-B064-F646-954A-277E8D659D34}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -929,31 +1191,31 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -967,7 +1229,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -996,7 +1258,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1025,7 +1287,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>12.8</v>
@@ -1050,6 +1312,151 @@
       </c>
       <c r="I4">
         <v>0.43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>10.8</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>84.6</v>
+      </c>
+      <c r="F5">
+        <v>42.5</v>
+      </c>
+      <c r="G5">
+        <v>1.24</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>11.98</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>84.6</v>
+      </c>
+      <c r="F6">
+        <v>42.5</v>
+      </c>
+      <c r="G6">
+        <v>1.24</v>
+      </c>
+      <c r="H6">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I6">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>10.5</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>84.6</v>
+      </c>
+      <c r="F7">
+        <v>42.5</v>
+      </c>
+      <c r="G7">
+        <v>1.24</v>
+      </c>
+      <c r="H7">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I7">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>84.6</v>
+      </c>
+      <c r="F8">
+        <v>42.5</v>
+      </c>
+      <c r="G8">
+        <v>1.24</v>
+      </c>
+      <c r="H8">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I8">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <v>9.17</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>84.6</v>
+      </c>
+      <c r="F9">
+        <v>42.5</v>
+      </c>
+      <c r="G9">
+        <v>1.24</v>
+      </c>
+      <c r="H9">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="I9">
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -1061,7 +1468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774F099D-606A-354D-9FEF-45FAE806DF04}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1085,72 +1492,72 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>0.56000000000000005</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>0.46926400000000001</v>
@@ -1165,7 +1572,7 @@
         <v>7.825E-2</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J2">
         <v>2.2501340000000001</v>
@@ -1180,7 +1587,7 @@
         <v>0.37675500000000001</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O2">
         <v>40.514409999999998</v>
@@ -1197,16 +1604,16 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>0.44530500000000001</v>
@@ -1221,7 +1628,7 @@
         <v>5.2609999999999997E-2</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J3">
         <v>2.1193759999999999</v>
@@ -1236,7 +1643,7 @@
         <v>0.23959800000000001</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O3">
         <v>40.495780000000003</v>
@@ -1253,16 +1660,16 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>2E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>0.37559100000000001</v>
@@ -1277,7 +1684,7 @@
         <v>3.1410000000000001E-3</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J4">
         <v>1.826109</v>
@@ -1292,7 +1699,7 @@
         <v>1.5114000000000001E-2</v>
       </c>
       <c r="N4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O4">
         <v>37.894750000000002</v>
@@ -1309,16 +1716,16 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>2E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>0.422315</v>
@@ -1333,7 +1740,7 @@
         <v>3.0230000000000001E-3</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J5">
         <v>2.4436909999999998</v>
@@ -1348,7 +1755,7 @@
         <v>1.4551E-2</v>
       </c>
       <c r="N5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O5">
         <v>22.6083</v>
@@ -1365,16 +1772,16 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
       </c>
       <c r="C6">
         <v>2E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>0.26783000000000001</v>
@@ -1389,7 +1796,7 @@
         <v>3.0479999999999999E-3</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J6">
         <v>1.6524460000000001</v>
@@ -1404,7 +1811,7 @@
         <v>1.4671E-2</v>
       </c>
       <c r="N6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O6">
         <v>35.471089999999997</v>
@@ -1421,16 +1828,16 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>1.5373619999999999</v>
@@ -1445,7 +1852,7 @@
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J7">
         <v>7.5076039999999997</v>
@@ -1460,7 +1867,7 @@
         <v>1.4933E-2</v>
       </c>
       <c r="N7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="O7">
         <v>14.00427</v>

</xml_diff>